<commit_message>
Edits from DQC meeting May 17, 2016. Add additional elements to rules 13, 14, 15, add additional constraints to rule 5 and rule 15. Edit MD files to show status of Public review.
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0013/DQC_0013_ListOfElements_V2.xlsx
+++ b/docs/DQC_US_0013/DQC_0013_ListOfElements_V2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26230"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="77">
   <si>
     <t>originalReleaseVersion</t>
   </si>
@@ -220,6 +223,54 @@
   </si>
   <si>
     <t>Percentage of the difference between reported income tax expense (benefit) and expected income tax expense (benefit) computed by applying the domestic federal statutory income tax rates to pretax income (loss) from continuing operations attributable to impairment loss.</t>
+  </si>
+  <si>
+    <t>Effective Income Tax Rate Reconciliation, Deduction, Employee Stock Ownership Plan Dividend, Percent</t>
+  </si>
+  <si>
+    <t>EffectiveIncomeTaxRateReconciliationDeductionsEmployeeStockOwnershipPlanDividends</t>
+  </si>
+  <si>
+    <t>Percentage of the difference between reported income tax expense (benefit) and expected income tax expense (benefit) computed by applying the domestic federal statutory income tax rates to pretax income (loss) from continuing operations attributable to deduction for dividend paid to employee stock ownership plan.</t>
+  </si>
+  <si>
+    <t>&gt; 1</t>
+  </si>
+  <si>
+    <t>Effective Income Tax Rate Reconciliation, Nondeductible Expense, Meals and Entertainment, Percent</t>
+  </si>
+  <si>
+    <t>EffectiveIncomeTaxRateReconciliationNondeductibleExpenseMealsAndEntertainment</t>
+  </si>
+  <si>
+    <t>Percentage of the difference between reported income tax expense (benefit) and expected income tax expense (benefit) computed by applying the domestic federal statutory income tax rates to pretax income (loss) from continuing operations attributable to meals and entertainment expense.</t>
+  </si>
+  <si>
+    <t>Effective Income Tax Rate Reconciliation, Deduction, Extraterritorial Income Exclusion, Percent</t>
+  </si>
+  <si>
+    <t>EffectiveIncomeTaxRateReconciliationDeductionsExtraterritorialIncomeExclusion</t>
+  </si>
+  <si>
+    <t>Percentage of the difference between reported income tax expense (benefit) and the expected income tax expense (benefit) computed by applying the domestic federal statutory income tax rates to pretax income (loss) from continuing operations attributable to deduction for extraterritorial income exclusion.</t>
+  </si>
+  <si>
+    <t>Effective Income Tax Rate Reconciliation, Nondeductible Expense, Charitable Contributions, Percent</t>
+  </si>
+  <si>
+    <t>EffectiveIncomeTaxRateReconciliationNondeductibleExpenseCharitableContributions</t>
+  </si>
+  <si>
+    <t>Percentage of the difference between reported income tax expense (benefit) and expected income tax expense (benefit) computed by applying the domestic federal statutory income tax rates to pretax income (loss) from continuing operations attributable to charitable contributions expense.</t>
+  </si>
+  <si>
+    <t>Effective Income Tax Rate Reconciliation, Repatriation Foreign Earnings, Jobs Creation Act of 2004, Percent</t>
+  </si>
+  <si>
+    <t>EffectiveIncomeTaxRateReconciliationRepatriationForeignEarningsJobsCreationActOf2004</t>
+  </si>
+  <si>
+    <t>Percentage of the difference between reported income tax expense (benefit) and expected income tax expense (benefit) computed by applying the domestic federal statutory income tax rates to pretax income (loss) from continuing operations attributable to the temporary incentive for U.S. entities to repatriate accumulated foreign earnings under the American Jobs Creation Act of 2004.</t>
   </si>
 </sst>
 </file>
@@ -575,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1124,45 +1175,165 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="K21" s="10"/>
+    <row r="17" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6">
+        <v>3001</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="6">
+        <v>3002</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3439</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3440</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="6">
+        <v>3441</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>

</xml_diff>

<commit_message>
Correct precondition criteria for rule 13
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0013/DQC_0013_ListOfElements_V2.xlsx
+++ b/docs/DQC_US_0013/DQC_0013_ListOfElements_V2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22640" yWindow="960" windowWidth="28560" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="6040" yWindow="1060" windowWidth="28560" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="76">
   <si>
     <t>originalReleaseVersion</t>
   </si>
@@ -232,9 +232,6 @@
   </si>
   <si>
     <t>Percentage of the difference between reported income tax expense (benefit) and expected income tax expense (benefit) computed by applying the domestic federal statutory income tax rates to pretax income (loss) from continuing operations attributable to deduction for dividend paid to employee stock ownership plan.</t>
-  </si>
-  <si>
-    <t>&gt; 1</t>
   </si>
   <si>
     <t>Effective Income Tax Rate Reconciliation, Nondeductible Expense, Meals and Entertainment, Percent</t>
@@ -626,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17:K21"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1224,19 +1221,19 @@
         <v>13</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1256,19 +1253,19 @@
         <v>13</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1288,19 +1285,19 @@
         <v>13</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1320,19 +1317,19 @@
         <v>13</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K21" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>